<commit_message>
Removed some outliers. Created a smaller dataset to see if it'll improve our model.
</commit_message>
<xml_diff>
--- a/ModelMetrics.xlsx
+++ b/ModelMetrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crystalcontreras/Desktop/DePaul/2021Spring/DSC423-DataAnalysis-Regression/DSC423FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C036FA0E-A177-E041-B7BA-F5D8C8A214C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C2C16B-AB7F-9444-A584-D1A23C2EBEF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2060" windowWidth="16020" windowHeight="11560" xr2:uid="{C21F6298-26AD-004F-BF92-3BD1598CAE96}"/>
+    <workbookView xWindow="9000" yWindow="6880" windowWidth="16580" windowHeight="9120" xr2:uid="{C21F6298-26AD-004F-BF92-3BD1598CAE96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Comparing Models</t>
   </si>
@@ -51,9 +51,6 @@
     <t>lowest</t>
   </si>
   <si>
-    <t>Standardized Estimates for:</t>
-  </si>
-  <si>
     <t>EMP_VAR_RATE</t>
   </si>
   <si>
@@ -72,12 +69,6 @@
     <t>NR_EMPLOYED</t>
   </si>
   <si>
-    <t>Backwards Selection Method</t>
-  </si>
-  <si>
-    <t>Stepwise Selection Method</t>
-  </si>
-  <si>
     <t>Parameter Estimates</t>
   </si>
   <si>
@@ -103,6 +94,21 @@
   </si>
   <si>
     <t>Stepwise</t>
+  </si>
+  <si>
+    <t>(Most Influential Predictor) Standardized Estimates for:</t>
+  </si>
+  <si>
+    <t>Backwards Selection Method (M1)</t>
+  </si>
+  <si>
+    <t>Stepwise Selection Method (M2)</t>
+  </si>
+  <si>
+    <t>Backwards w/removed some outliers (M3)</t>
+  </si>
+  <si>
+    <t>M4</t>
   </si>
 </sst>
 </file>
@@ -145,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -154,6 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,35 +475,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099E10C2-5918-AE4B-B455-53FDC71C0C78}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -506,14 +519,20 @@
       <c r="C4">
         <v>0.2697</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>0.26469999999999999</v>
       </c>
       <c r="E4">
         <v>0.26369999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>0.27850000000000003</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.28949999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -523,14 +542,20 @@
       <c r="C5">
         <v>1371.0329999999999</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>1334.452</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>1336.414</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>1248.691</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1193.5999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -540,14 +565,20 @@
       <c r="C6">
         <v>1606.434</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>1394.8109999999999</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>1390.7380000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>1309</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1253.8699999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -557,21 +588,27 @@
       <c r="C7">
         <v>971.37390000000005</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>1314.452</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>945.99239999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>1004.8814</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1050.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
       </c>
       <c r="C10">
         <v>-0.76629999999999998</v>
@@ -579,32 +616,36 @@
       <c r="D10" s="2">
         <v>-0.81130000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>0.44879999999999998</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.4536</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="4">
+        <v>0.12690000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>-0.18790000000000001</v>
       </c>
-      <c r="E12" s="2">
-        <v>0.97399999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="4">
+        <v>-0.10580000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>3.0800000000000001E-2</v>
@@ -612,32 +653,33 @@
       <c r="D13">
         <v>0.13439999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>7.0099999999999996E-2</v>
       </c>
-      <c r="E14" s="2">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="E14" s="4">
+        <v>-0.52229999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <v>-134.19999999999999</v>
@@ -648,7 +690,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>4.8300000000000001E-3</v>
@@ -659,7 +701,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>-0.92190000000000005</v>
@@ -667,7 +709,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>1.4043000000000001</v>
@@ -675,7 +717,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21">
         <v>6.4899999999999999E-2</v>
@@ -686,7 +728,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D22">
         <v>1.2008000000000001</v>
@@ -697,7 +739,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D23">
         <v>2.5969000000000002</v>
@@ -708,7 +750,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24">
         <v>-0.41220000000000001</v>
@@ -716,7 +758,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D25">
         <v>0.74390000000000001</v>
@@ -727,7 +769,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>0.66439999999999999</v>
@@ -735,7 +777,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27">
         <v>-1.24E-2</v>
@@ -743,7 +785,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D28">
         <v>1.4984</v>

</xml_diff>

<commit_message>
Generated predictions and confusion matrix. Updated analysis and stats.
</commit_message>
<xml_diff>
--- a/ModelMetrics.xlsx
+++ b/ModelMetrics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crystalcontreras/Desktop/DePaul/2021Spring/DSC423-DataAnalysis-Regression/DSC423FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C2C16B-AB7F-9444-A584-D1A23C2EBEF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78609828-44D6-5542-8F54-F7409148BDAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="6880" windowWidth="16580" windowHeight="9120" xr2:uid="{C21F6298-26AD-004F-BF92-3BD1598CAE96}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{C21F6298-26AD-004F-BF92-3BD1598CAE96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Comparing Models</t>
   </si>
@@ -108,14 +109,74 @@
     <t>Backwards w/removed some outliers (M3)</t>
   </si>
   <si>
-    <t>M4</t>
+    <t>bank_small Backwards (M5)</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Backwards w/more removed outliers (M4)</t>
+  </si>
+  <si>
+    <t>bank_small Stepwise (M6)</t>
+  </si>
+  <si>
+    <t>bank_small2 Backwards (M7)</t>
+  </si>
+  <si>
+    <t>bank_small2 Stepwise (M8)</t>
+  </si>
+  <si>
+    <t>bank_small2 Full Model</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>M10 (removed outliers)</t>
+  </si>
+  <si>
+    <t>642?</t>
+  </si>
+  <si>
+    <t>M11 (removed more outliers)</t>
+  </si>
+  <si>
+    <t>M12 (stepwise on training set)</t>
+  </si>
+  <si>
+    <t>M13 (backwards on training set)</t>
+  </si>
+  <si>
+    <t>LR (H0)</t>
+  </si>
+  <si>
+    <t>classification table</t>
+  </si>
+  <si>
+    <t>prob level</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>specificity</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>sensitivity (Y=1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +185,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="9"/>
       <name val="Calibri"/>
@@ -139,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -147,11 +224,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -161,6 +275,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,24 +624,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099E10C2-5918-AE4B-B455-53FDC71C0C78}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
@@ -506,295 +657,841 @@
         <v>26</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="I3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3090</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3090</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3090</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3079</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1373</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1373</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1090</v>
+      </c>
+      <c r="M4" s="10">
+        <v>1090</v>
+      </c>
+      <c r="N4" s="12">
+        <v>1090</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1090</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1079</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1070</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3">
+        <v>9</v>
+      </c>
+      <c r="H5" s="6">
+        <v>13</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="3">
+        <v>54</v>
+      </c>
+      <c r="M5" s="10">
+        <v>12</v>
+      </c>
+      <c r="N5" s="12">
+        <v>10</v>
+      </c>
+      <c r="O5" s="3">
+        <v>11</v>
+      </c>
+      <c r="P5" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>11</v>
+      </c>
+      <c r="R5" s="5">
+        <v>7</v>
+      </c>
+      <c r="S5" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>0.2697</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D6" s="4">
         <v>0.26469999999999999</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <v>0.26369999999999999</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>0.27850000000000003</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G6" s="2">
         <v>0.28949999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="H6" s="7">
+        <v>0.43230000000000002</v>
+      </c>
+      <c r="I6">
+        <v>0.34539999999999998</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>0.45379999999999998</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0.44490000000000002</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.44019999999999998</v>
+      </c>
+      <c r="O6" s="14">
+        <v>0.44209999999999999</v>
+      </c>
+      <c r="P6" s="14">
+        <v>0.48430000000000001</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0.51</v>
+      </c>
+      <c r="R6" s="14">
+        <v>0.53</v>
+      </c>
+      <c r="S6" s="17">
+        <v>0.53769999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C7">
         <v>1371.0329999999999</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D7" s="4">
         <v>1334.452</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E7" s="4">
         <v>1336.414</v>
       </c>
-      <c r="F5">
+      <c r="F7">
         <v>1248.691</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G7" s="2">
         <v>1193.5999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="H7" s="7">
+        <v>850.78</v>
+      </c>
+      <c r="I7">
+        <v>1024</v>
+      </c>
+      <c r="K7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>815.37</v>
+      </c>
+      <c r="M7" s="11">
+        <v>781.14</v>
+      </c>
+      <c r="N7" s="4">
+        <v>786.36</v>
+      </c>
+      <c r="O7" s="3">
+        <v>784.6</v>
+      </c>
+      <c r="P7" s="3">
+        <v>690</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>623</v>
+      </c>
+      <c r="R7" s="15">
+        <v>360</v>
+      </c>
+      <c r="S7" s="16">
+        <v>355.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>1606.434</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D8" s="4">
         <v>1394.8109999999999</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E8" s="4">
         <v>1390.7380000000001</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>1309</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G8" s="2">
         <v>1253.8699999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="H8" s="7">
+        <v>923.9</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1040</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1010.135</v>
+      </c>
+      <c r="M8" s="10">
+        <v>846</v>
+      </c>
+      <c r="N8" s="5">
+        <v>841.29399999999998</v>
+      </c>
+      <c r="O8" s="5">
+        <v>844.57</v>
+      </c>
+      <c r="P8" s="3">
+        <v>750</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>682.95</v>
+      </c>
+      <c r="R8" s="16">
+        <v>395.78</v>
+      </c>
+      <c r="S8" s="15">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>971.37390000000005</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D9" s="4">
         <v>1314.452</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E9" s="4">
         <v>945.99239999999998</v>
       </c>
-      <c r="F7">
+      <c r="F9">
         <v>1004.8814</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G9" s="2">
         <v>1050.45</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="H9" s="8">
+        <v>777</v>
+      </c>
+      <c r="I9" s="3">
+        <v>581.77</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="3">
+        <v>659.29</v>
+      </c>
+      <c r="M9" s="13">
+        <v>641.5</v>
+      </c>
+      <c r="N9" s="12">
+        <v>632.29899999999998</v>
+      </c>
+      <c r="O9" s="3">
+        <v>636</v>
+      </c>
+      <c r="P9" s="3">
+        <v>714.5</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>772.8</v>
+      </c>
+      <c r="R9" s="15">
+        <v>485</v>
+      </c>
+      <c r="S9" s="16">
+        <v>495.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>-0.76629999999999998</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D12" s="2">
         <v>-0.81130000000000002</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="C13">
         <v>0.44879999999999998</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D13" s="2">
         <v>0.4536</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E13" s="4">
         <v>0.12690000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C14">
         <v>-0.18790000000000001</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E14" s="4">
         <v>-0.10580000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>3.0800000000000001E-2</v>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>0.13439999999999999</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>7.0099999999999996E-2</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E16" s="4">
         <v>-0.52229999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17">
-        <v>-134.19999999999999</v>
-      </c>
-      <c r="E17">
-        <v>60.76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18">
-        <v>4.8300000000000001E-3</v>
-      </c>
-      <c r="E18">
-        <v>4.7999999999999996E-3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D19">
-        <v>-0.92190000000000005</v>
+        <v>-134.19999999999999</v>
+      </c>
+      <c r="E19">
+        <v>60.76</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>1.4043000000000001</v>
+        <v>4.8300000000000001E-3</v>
+      </c>
+      <c r="E20">
+        <v>4.7999999999999996E-3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D21">
-        <v>6.4899999999999999E-2</v>
-      </c>
-      <c r="E21">
-        <v>4.8500000000000001E-2</v>
+        <v>-0.92190000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D22">
-        <v>1.2008000000000001</v>
-      </c>
-      <c r="E22">
-        <v>1.0821000000000001</v>
+        <v>1.4043000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D23">
-        <v>2.5969000000000002</v>
+        <v>6.4899999999999999E-2</v>
       </c>
       <c r="E23">
-        <v>2.0956000000000001</v>
+        <v>4.8500000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="D24">
+        <v>1.2008000000000001</v>
       </c>
       <c r="E24">
-        <v>-0.41220000000000001</v>
+        <v>1.0821000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>0.74390000000000001</v>
+        <v>2.5969000000000002</v>
       </c>
       <c r="E25">
-        <v>1.2212000000000001</v>
+        <v>2.0956000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26">
-        <v>0.66439999999999999</v>
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>-0.41220000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <v>0.74390000000000001</v>
       </c>
       <c r="E27">
-        <v>-1.24E-2</v>
+        <v>1.2212000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>0.66439999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29">
+        <v>-1.24E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>20</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>1.4984</v>
       </c>
-      <c r="E28">
+      <c r="E30">
         <v>1.5582</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD7D112-5715-874A-99C1-9AE141E3FBAB}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.1</v>
+      </c>
+      <c r="D4">
+        <v>98.2</v>
+      </c>
+      <c r="E4">
+        <v>74</v>
+      </c>
+      <c r="F4">
+        <f>SUM(D4:E4)</f>
+        <v>172.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>A4+0.05</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="D5">
+        <v>96.9</v>
+      </c>
+      <c r="E5">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F18" si="0">SUM(D5:E5)</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" ref="A6:A20" si="1">A5+0.05</f>
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>93.3</v>
+      </c>
+      <c r="E6">
+        <v>79</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>172.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="D7">
+        <v>92.8</v>
+      </c>
+      <c r="E7">
+        <v>79.7</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>172.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="D8">
+        <v>91.5</v>
+      </c>
+      <c r="E8">
+        <v>82.1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>173.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>0.35</v>
+      </c>
+      <c r="D9">
+        <v>89.7</v>
+      </c>
+      <c r="E9">
+        <v>84.7</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>174.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="D10">
+        <v>86.1</v>
+      </c>
+      <c r="E10">
+        <v>86.6</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>172.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="D11">
+        <v>85.7</v>
+      </c>
+      <c r="E11">
+        <v>88.3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="D12">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="E12">
+        <v>89.5</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>171.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="D13">
+        <v>78</v>
+      </c>
+      <c r="E13">
+        <v>91.4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>169.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="D14">
+        <v>75.3</v>
+      </c>
+      <c r="E14">
+        <v>93.1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>168.39999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="D15">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E15">
+        <v>94.5</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>164.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="D16">
+        <v>65.5</v>
+      </c>
+      <c r="E16">
+        <v>95.9</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>161.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="D17">
+        <v>61.4</v>
+      </c>
+      <c r="E17">
+        <v>96.7</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>158.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="D18">
+        <v>56.1</v>
+      </c>
+      <c r="E18">
+        <v>97.1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>153.19999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Renamed docx files to avoid merge conflicts.  Wrapped up Analysis with subset stats.
</commit_message>
<xml_diff>
--- a/ModelMetrics.xlsx
+++ b/ModelMetrics.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crystalcontreras/Desktop/DePaul/2021Spring/DSC423-DataAnalysis-Regression/DSC423FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78609828-44D6-5542-8F54-F7409148BDAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8D5D01-792F-4344-9749-1A37E9CC73AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{C21F6298-26AD-004F-BF92-3BD1598CAE96}"/>
+    <workbookView xWindow="-20" yWindow="1160" windowWidth="25600" windowHeight="9800" xr2:uid="{C21F6298-26AD-004F-BF92-3BD1598CAE96}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="ModelComparison" sheetId="1" r:id="rId1"/>
+    <sheet name="ClassificationTable" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Comparing Models</t>
   </si>
@@ -170,6 +170,21 @@
   </si>
   <si>
     <t>sensitivity (Y=1)</t>
+  </si>
+  <si>
+    <t>M16 (Stepwise on bank_new2 training set)</t>
+  </si>
+  <si>
+    <t>Keerthi's Model</t>
+  </si>
+  <si>
+    <t>FINAL MODEL WINNER: M12</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>&lt;0.0001</t>
   </si>
 </sst>
 </file>
@@ -265,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -309,6 +324,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099E10C2-5918-AE4B-B455-53FDC71C0C78}">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="R3" sqref="K3:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,12 +659,17 @@
     <col min="15" max="15" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="R2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
@@ -683,14 +709,20 @@
       <c r="Q3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="20" t="s">
         <v>39</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="T3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
@@ -733,11 +765,14 @@
       <c r="Q4" s="3">
         <v>1070</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" s="20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="V4" s="3">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
@@ -781,14 +816,17 @@
       <c r="Q5" s="3">
         <v>11</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="21">
         <v>7</v>
       </c>
       <c r="S5" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -798,7 +836,7 @@
       <c r="C6">
         <v>0.2697</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>0.26469999999999999</v>
       </c>
       <c r="E6">
@@ -843,8 +881,11 @@
       <c r="S6" s="17">
         <v>0.53769999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V6">
+        <v>0.24129999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -854,7 +895,7 @@
       <c r="C7">
         <v>1371.0329999999999</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>1334.452</v>
       </c>
       <c r="E7" s="4">
@@ -900,7 +941,7 @@
         <v>355.86</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -913,7 +954,7 @@
       <c r="D8" s="4">
         <v>1394.8109999999999</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>1390.7380000000001</v>
       </c>
       <c r="F8">
@@ -957,7 +998,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -967,7 +1008,7 @@
       <c r="C9">
         <v>971.37390000000005</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>1314.452</v>
       </c>
       <c r="E9" s="4">
@@ -1014,12 +1055,23 @@
         <v>495.3</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>51</v>
+      </c>
+      <c r="R10" t="s">
+        <v>52</v>
+      </c>
+      <c r="V10">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1031,7 +1083,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1097,7 @@
         <v>0.12690000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1056,7 +1108,7 @@
         <v>-0.10580000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1068,7 +1120,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1216,7 +1268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD7D112-5715-874A-99C1-9AE141E3FBAB}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Team evaluation document & source report on dataset.
</commit_message>
<xml_diff>
--- a/ModelMetrics.xlsx
+++ b/ModelMetrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crystalcontreras/Desktop/DePaul/2021Spring/DSC423-DataAnalysis-Regression/DSC423FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8D5D01-792F-4344-9749-1A37E9CC73AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F14FCD-8BF6-A34A-B55B-32882EC940FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="1160" windowWidth="25600" windowHeight="9800" xr2:uid="{C21F6298-26AD-004F-BF92-3BD1598CAE96}"/>
+    <workbookView xWindow="3300" yWindow="3560" windowWidth="22140" windowHeight="12380" activeTab="1" xr2:uid="{C21F6298-26AD-004F-BF92-3BD1598CAE96}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelComparison" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Comparing Models</t>
   </si>
@@ -160,15 +160,9 @@
     <t>prob level</t>
   </si>
   <si>
-    <t>correct</t>
-  </si>
-  <si>
     <t>specificity</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
     <t>sensitivity (Y=1)</t>
   </si>
   <si>
@@ -185,6 +179,9 @@
   </si>
   <si>
     <t>&lt;0.0001</t>
+  </si>
+  <si>
+    <t>sensitivity + specificity</t>
   </si>
 </sst>
 </file>
@@ -280,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,17 +316,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099E10C2-5918-AE4B-B455-53FDC71C0C78}">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="R3" sqref="K3:R10"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S1" sqref="R1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,6 +657,7 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="13" max="13" width="13.1640625" customWidth="1"/>
     <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="20" max="20" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
@@ -666,7 +667,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="R2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -709,17 +710,17 @@
       <c r="Q3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="18" t="s">
         <v>39</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>40</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -765,7 +766,7 @@
       <c r="Q4" s="3">
         <v>1070</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="18" t="s">
         <v>37</v>
       </c>
       <c r="V4" s="3">
@@ -816,7 +817,7 @@
       <c r="Q5" s="3">
         <v>11</v>
       </c>
-      <c r="R5" s="21">
+      <c r="R5" s="19">
         <v>7</v>
       </c>
       <c r="S5" s="3">
@@ -1057,10 +1058,10 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="K10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="V10">
         <v>0.91</v>
@@ -1266,284 +1267,288 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD7D112-5715-874A-99C1-9AE141E3FBAB}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" style="21" customWidth="1"/>
+    <col min="2" max="2" width="2.5" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="21"/>
+    <col min="5" max="5" width="17.5" style="21" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="E3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
         <v>0.1</v>
       </c>
-      <c r="D4">
+      <c r="C4" s="21">
         <v>98.2</v>
       </c>
-      <c r="E4">
+      <c r="D4" s="21">
         <v>74</v>
       </c>
-      <c r="F4">
-        <f>SUM(D4:E4)</f>
+      <c r="E4" s="21">
+        <f>SUM(C4:D4)</f>
         <v>172.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="21">
         <f>A4+0.05</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="D5">
+      <c r="C5" s="21">
         <v>96.9</v>
       </c>
-      <c r="E5">
+      <c r="D5" s="21">
         <v>77.099999999999994</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F18" si="0">SUM(D5:E5)</f>
+      <c r="E5" s="21">
+        <f t="shared" ref="E5:E18" si="0">SUM(C5:D5)</f>
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <f t="shared" ref="A6:A20" si="1">A5+0.05</f>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="21">
+        <f t="shared" ref="A6:A18" si="1">A5+0.05</f>
         <v>0.2</v>
       </c>
-      <c r="D6">
+      <c r="C6" s="21">
         <v>93.3</v>
       </c>
-      <c r="E6">
+      <c r="D6" s="21">
         <v>79</v>
       </c>
-      <c r="F6">
+      <c r="E6" s="21">
         <f t="shared" si="0"/>
         <v>172.3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="21">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="D7">
+      <c r="C7" s="21">
         <v>92.8</v>
       </c>
-      <c r="E7">
+      <c r="D7" s="21">
         <v>79.7</v>
       </c>
-      <c r="F7">
+      <c r="E7" s="21">
         <f t="shared" si="0"/>
         <v>172.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="21">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="D8">
+      <c r="C8" s="21">
         <v>91.5</v>
       </c>
-      <c r="E8">
+      <c r="D8" s="21">
         <v>82.1</v>
       </c>
-      <c r="F8">
+      <c r="E8" s="21">
         <f t="shared" si="0"/>
         <v>173.6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="21">
         <f t="shared" si="1"/>
         <v>0.35</v>
       </c>
-      <c r="D9">
+      <c r="C9" s="21">
         <v>89.7</v>
       </c>
-      <c r="E9">
+      <c r="D9" s="21">
         <v>84.7</v>
       </c>
-      <c r="F9" s="2">
+      <c r="E9" s="22">
         <f t="shared" si="0"/>
         <v>174.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="21">
         <f t="shared" si="1"/>
         <v>0.39999999999999997</v>
       </c>
-      <c r="D10">
+      <c r="C10" s="21">
         <v>86.1</v>
       </c>
-      <c r="E10">
+      <c r="D10" s="21">
         <v>86.6</v>
       </c>
-      <c r="F10">
+      <c r="E10" s="21">
         <f t="shared" si="0"/>
         <v>172.7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="21">
         <f t="shared" si="1"/>
         <v>0.44999999999999996</v>
       </c>
-      <c r="D11">
+      <c r="C11" s="21">
         <v>85.7</v>
       </c>
-      <c r="E11">
+      <c r="D11" s="21">
         <v>88.3</v>
       </c>
-      <c r="F11">
+      <c r="E11" s="21">
         <f t="shared" si="0"/>
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="21">
         <f t="shared" si="1"/>
         <v>0.49999999999999994</v>
       </c>
-      <c r="D12">
+      <c r="C12" s="21">
         <v>81.599999999999994</v>
       </c>
-      <c r="E12">
+      <c r="D12" s="21">
         <v>89.5</v>
       </c>
-      <c r="F12">
+      <c r="E12" s="21">
         <f t="shared" si="0"/>
         <v>171.1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="21">
         <f t="shared" si="1"/>
         <v>0.54999999999999993</v>
       </c>
-      <c r="D13">
+      <c r="C13" s="21">
         <v>78</v>
       </c>
-      <c r="E13">
+      <c r="D13" s="21">
         <v>91.4</v>
       </c>
-      <c r="F13">
+      <c r="E13" s="21">
         <f t="shared" si="0"/>
         <v>169.4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="21">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="D14">
+      <c r="C14" s="21">
         <v>75.3</v>
       </c>
-      <c r="E14">
+      <c r="D14" s="21">
         <v>93.1</v>
       </c>
-      <c r="F14">
+      <c r="E14" s="21">
         <f t="shared" si="0"/>
         <v>168.39999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="21">
         <f t="shared" si="1"/>
         <v>0.65</v>
       </c>
-      <c r="D15">
+      <c r="C15" s="21">
         <v>70.400000000000006</v>
       </c>
-      <c r="E15">
+      <c r="D15" s="21">
         <v>94.5</v>
       </c>
-      <c r="F15">
+      <c r="E15" s="21">
         <f t="shared" si="0"/>
         <v>164.9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="21">
         <f t="shared" si="1"/>
         <v>0.70000000000000007</v>
       </c>
-      <c r="D16">
+      <c r="C16" s="21">
         <v>65.5</v>
       </c>
-      <c r="E16">
+      <c r="D16" s="21">
         <v>95.9</v>
       </c>
-      <c r="F16">
+      <c r="E16" s="21">
         <f t="shared" si="0"/>
         <v>161.4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="21">
         <f t="shared" si="1"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="D17">
+      <c r="C17" s="21">
         <v>61.4</v>
       </c>
-      <c r="E17">
+      <c r="D17" s="21">
         <v>96.7</v>
       </c>
-      <c r="F17">
+      <c r="E17" s="21">
         <f t="shared" si="0"/>
         <v>158.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="21">
         <f t="shared" si="1"/>
         <v>0.80000000000000016</v>
       </c>
-      <c r="D18">
+      <c r="C18" s="21">
         <v>56.1</v>
       </c>
-      <c r="E18">
+      <c r="D18" s="21">
         <v>97.1</v>
       </c>
-      <c r="F18">
+      <c r="E18" s="21">
         <f t="shared" si="0"/>
         <v>153.19999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>